<commit_message>
adding results and cleaning
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\syazdipour\sources\thesis\text-to-sql-thesis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shyaz\sources\thesis\text-to-sql-thesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC0B8AF8-E18B-4CE7-A0A8-BD47D415F456}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{665258ED-15BB-4762-89BD-870827C2FAAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="30">
   <si>
     <t>select</t>
   </si>
@@ -123,13 +123,19 @@
   <si>
     <t>Seq2Seq</t>
   </si>
+  <si>
+    <t>ChatGPT 3.5</t>
+  </si>
+  <si>
+    <t>ChatGPT 4</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="167" formatCode="m/yyyy"/>
+    <numFmt numFmtId="164" formatCode="m/yyyy"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -163,17 +169,17 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
-      <numFmt numFmtId="167" formatCode="m/yyyy"/>
+      <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
+      <numFmt numFmtId="164" formatCode="m/yyyy"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1693,9 +1699,9 @@
           </c:marker>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>Sheet1!$A$2:$B$12</c:f>
+              <c:f>Sheet1!$A$2:$B$14</c:f>
               <c:multiLvlStrCache>
-                <c:ptCount val="11"/>
+                <c:ptCount val="13"/>
                 <c:lvl>
                   <c:pt idx="0">
                     <c:v>Seq2Seq</c:v>
@@ -1729,6 +1735,12 @@
                   </c:pt>
                   <c:pt idx="10">
                     <c:v>T5-3B+PICARD</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>ChatGPT 3.5</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>ChatGPT 4</c:v>
                   </c:pt>
                 </c:lvl>
                 <c:lvl>
@@ -1765,16 +1777,22 @@
                   <c:pt idx="10">
                     <c:v>7/2021</c:v>
                   </c:pt>
+                  <c:pt idx="11">
+                    <c:v>2/2023</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>3/2023</c:v>
+                  </c:pt>
                 </c:lvl>
               </c:multiLvlStrCache>
             </c:multiLvlStrRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$2:$C$12</c:f>
+              <c:f>Sheet1!$C$2:$C$14</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>4.8</c:v>
                 </c:pt>
@@ -1807,6 +1825,12 @@
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>71.900000000000006</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>81.3</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>85.2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3710,13 +3734,13 @@
       <xdr:col>3</xdr:col>
       <xdr:colOff>152401</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>138111</xdr:rowOff>
+      <xdr:rowOff>138110</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
       <xdr:colOff>466725</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>38099</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3748,9 +3772,9 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{EFBC020F-42E8-431D-B7C1-D4BC20392AE0}" name="Table1" displayName="Table1" ref="A1:C1048574" totalsRowShown="0">
   <autoFilter ref="A1:C1048574" xr:uid="{EFBC020F-42E8-431D-B7C1-D4BC20392AE0}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{56D94D08-18F9-48EB-8A66-3CEFF1FE0481}" name="Submit" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{56D94D08-18F9-48EB-8A66-3CEFF1FE0481}" name="Submit" dataDxfId="1"/>
     <tableColumn id="2" xr3:uid="{899F5B55-16CB-49E1-A2BB-9E1AEC71C6F5}" name="Model"/>
-    <tableColumn id="3" xr3:uid="{0D4FEC25-0651-47A4-B251-C11BE25BE5CC}" name="ESM Test no value" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{0D4FEC25-0651-47A4-B251-C11BE25BE5CC}" name="ESM Test no value" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4479,10 +4503,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C51889CC-E4C3-4FCC-9571-901DC145E6C1}">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4624,6 +4648,28 @@
         <v>71.900000000000006</v>
       </c>
     </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="2">
+        <v>44958</v>
+      </c>
+      <c r="B13" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13" s="1">
+        <v>81.3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="2">
+        <v>44986</v>
+      </c>
+      <c r="B14" t="s">
+        <v>29</v>
+      </c>
+      <c r="C14" s="1">
+        <v>85.2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>